<commit_message>
added first draft of project plan
</commit_message>
<xml_diff>
--- a/ProjectPlan/gantt-chart_L.xlsx
+++ b/ProjectPlan/gantt-chart_L.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fazi/Desktop/irp-acse-fk4517/ProjectPlan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C3B1F-FA2C-644F-9B24-630A45F323CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6EA855-8B4E-1C4B-A713-0B40931DE860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{321AA13A-52DF-024B-B440-65B5AD92623C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Literature Review</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Review Existing Visualization Libraries</t>
   </si>
   <si>
-    <t>Learn Further Library Design Principles</t>
-  </si>
-  <si>
     <t>Implement Basic Library Structure</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>Test Library</t>
   </si>
   <si>
-    <t>Review Summaries</t>
-  </si>
-  <si>
     <t>Write Independent Research Report</t>
   </si>
   <si>
@@ -90,6 +84,9 @@
   </si>
   <si>
     <t>Project Schedule</t>
+  </si>
+  <si>
+    <t>Review Best Practices</t>
   </si>
 </sst>
 </file>
@@ -261,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48894AB6-11CF-2845-B697-0BA8A722576F}">
-  <dimension ref="B1:R20"/>
+  <dimension ref="B1:R19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,9 +586,9 @@
     <col min="3" max="3" width="1.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
@@ -734,7 +731,7 @@
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="10"/>
@@ -814,7 +811,7 @@
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="10"/>
@@ -834,7 +831,7 @@
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="10"/>
@@ -874,7 +871,7 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -894,7 +891,7 @@
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="10"/>
@@ -907,14 +904,14 @@
       <c r="K15" s="10"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="10"/>
@@ -925,59 +922,59 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
       <c r="O16" s="6"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
+      <c r="B18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C19" s="12"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -990,27 +987,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
+      <c r="Q19" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>